<commit_message>
Multiple changes and optimizations
</commit_message>
<xml_diff>
--- a/assets/records_worksheet.xlsx
+++ b/assets/records_worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mholi\OneDrive\Documents\szpb-map\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743C8A90-EEBC-41CA-8418-0A6CC5CB7D98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4050A5-7C8F-4A80-8D13-3D914F218D65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="607" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="607" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -2445,7 +2445,7 @@
   <dimension ref="A1:I113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="F121" sqref="F121"/>
+      <selection activeCell="G111" sqref="G111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>